<commit_message>
ng: update pretas form
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Nigeria/june 2024/ng_lf_pretas_202406_2_resultat_fts.xlsx
+++ b/LF/PreTAS/Nigeria/june 2024/ng_lf_pretas_202406_2_resultat_fts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\PreTAS\Nigeria\june 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95E6B9E-5D21-420B-981E-BEC1BCA6B56D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C904091-C565-4E0E-AE69-49B8CD85A29B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="161">
   <si>
     <t>type</t>
   </si>
@@ -518,6 +518,9 @@
   </si>
   <si>
     <t>ng_lf_pretas_202406_2_fts_v2</t>
+  </si>
+  <si>
+    <t>barcode</t>
   </si>
 </sst>
 </file>
@@ -1070,11 +1073,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1399,7 +1402,7 @@
     </row>
     <row r="13" spans="1:15" s="16" customFormat="1" ht="31.5">
       <c r="A13" s="29" t="s">
-        <v>24</v>
+        <v>160</v>
       </c>
       <c r="B13" s="30" t="s">
         <v>25</v>
@@ -3426,7 +3429,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>